<commit_message>
Made some additions to the Gantt Chart
Added Risk Severity Key
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\Year 4\Capstone\Administration\Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1E332CE-6C0B-4227-8F34-765BC1590A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0A1FAF-5D33-47D5-B1D8-C17699C83550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C7C0535D-781E-4851-AAB9-D8919E2EA6F5}"/>
   </bookViews>
@@ -155,9 +155,6 @@
     <t>S1, Week 4</t>
   </si>
   <si>
-    <t>incomplete</t>
-  </si>
-  <si>
     <t>IPP Gate Review</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>S2, Week 7</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
 </sst>
 </file>
@@ -957,106 +957,106 @@
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="L2" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="N2" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="O2" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="P2" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="Q2" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="R2" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="S2" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="T2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="U2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="V2" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="W2" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="X2" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="Y2" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="AA2" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AA2" s="20" t="s">
+      <c r="AB2" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AC2" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AC2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="AD2" s="20" t="s">
+      <c r="AE2" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AF2" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AG2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="AJ2" s="20" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,13 +1696,13 @@
         <v>3</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J15" s="16"/>
       <c r="L15" s="19"/>
@@ -1792,13 +1792,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>38</v>
@@ -1844,7 +1844,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>16</v>
@@ -1855,8 +1855,8 @@
       <c r="H18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>39</v>
+      <c r="I18" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J18" s="12"/>
       <c r="L18" s="1"/>
@@ -1894,19 +1894,19 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="I19" s="7" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J19" s="8"/>
       <c r="L19" s="19"/>
@@ -1944,7 +1944,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>25</v>
@@ -1953,10 +1953,10 @@
         <v>4</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J20" s="12"/>
       <c r="L20" s="1"/>
@@ -1994,19 +1994,19 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>39</v>
+        <v>99</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J21" s="16"/>
       <c r="L21" s="19"/>
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
@@ -2053,10 +2053,10 @@
         <v>28</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J22" s="12"/>
       <c r="L22" s="30"/>
@@ -2094,19 +2094,19 @@
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>39</v>
+        <v>100</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J23" s="16"/>
       <c r="L23" s="19"/>
@@ -2144,19 +2144,19 @@
         <v>1</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="I24" s="7" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J24" s="8"/>
       <c r="L24" s="1"/>
@@ -2194,19 +2194,19 @@
         <v>1</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J25" s="10"/>
       <c r="L25" s="19"/>
@@ -2244,19 +2244,19 @@
         <v>1</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J26" s="8"/>
       <c r="L26" s="1"/>
@@ -2294,19 +2294,19 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>39</v>
+        <v>102</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J27" s="16"/>
       <c r="L27" s="1"/>
@@ -2338,13 +2338,13 @@
     <row r="28" spans="2:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>16</v>
@@ -2353,10 +2353,10 @@
         <v>28</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>39</v>
+        <v>101</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J28" s="12"/>
       <c r="L28" s="19"/>
@@ -2394,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>9</v>
@@ -2403,10 +2403,10 @@
         <v>28</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>39</v>
+        <v>98</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J29" s="12"/>
       <c r="L29" s="19"/>
@@ -2444,19 +2444,19 @@
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="J30" s="16"/>
       <c r="L30" s="1"/>
@@ -2494,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>25</v>
@@ -2503,10 +2503,10 @@
         <v>28</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>39</v>
+        <v>95</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J31" s="12"/>
       <c r="L31" s="19"/>
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>9</v>
@@ -2553,10 +2553,10 @@
         <v>28</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>39</v>
+        <v>95</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J32" s="12"/>
       <c r="L32" s="1"/>
@@ -2594,19 +2594,19 @@
         <v>1</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="I33" s="7" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J33" s="8"/>
       <c r="L33" s="19"/>
@@ -2644,19 +2644,19 @@
         <v>1</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J34" s="10"/>
       <c r="L34" s="30"/>
@@ -2694,19 +2694,19 @@
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J35" s="16"/>
       <c r="L35" s="19"/>
@@ -2744,19 +2744,19 @@
         <v>1</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J36" s="8"/>
       <c r="L36" s="1"/>
@@ -2794,7 +2794,7 @@
         <v>14</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>23</v>
@@ -2803,10 +2803,10 @@
         <v>4</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>39</v>
+        <v>66</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="J37" s="12"/>
       <c r="L37" s="19"/>
@@ -2844,19 +2844,19 @@
         <v>14</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J38" s="10"/>
       <c r="L38" s="1"/>

</xml_diff>